<commit_message>
Changes after Recovered data Aug172023
</commit_message>
<xml_diff>
--- a/TestData/TMTI0028216_VerifyNewJobForLOBOtherThanCF.xlsx
+++ b/TestData/TMTI0028216_VerifyNewJobForLOBOtherThanCF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E177DD70-B520-4F1B-BF23-878B0D2586E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D0A6A9-A72B-42C8-9686-28D0DF171CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23184" windowHeight="11388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>JobType</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Valuation Advisory</t>
+  </si>
+  <si>
+    <t>Lender Education</t>
   </si>
 </sst>
 </file>
@@ -303,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -431,6 +434,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -474,11 +488,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyFont="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyFont="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -839,7 +854,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,10 +885,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,6 +916,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>